<commit_message>
add more detail for de 14
</commit_message>
<xml_diff>
--- a/de14.xlsx
+++ b/de14.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gdrive\HATCOM_Chung chi tin hoc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\chtien18.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -439,16 +439,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>39688</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>370418</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>185209</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>296334</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>18521</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>31751</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>164042</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -471,8 +471,84 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8294688" y="1574271"/>
+          <a:off x="14909272" y="1124480"/>
           <a:ext cx="2413000" cy="2413000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>92604</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>622961</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>188496</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7064375" y="238125"/>
+          <a:ext cx="7409524" cy="3323809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>145521</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>39687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>508855</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>169449</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7117292" y="3611562"/>
+          <a:ext cx="5866667" cy="3304762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -834,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>